<commit_message>
Change example data so that one file does not have duplicate questionable results. Update tests accordingly.
</commit_message>
<xml_diff>
--- a/inst/extdata/SPAC_081599.xlsx
+++ b/inst/extdata/SPAC_081599.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/lsmith_nps_gov1/Documents/Documents/CCAL/imd-ccal/inst/extdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sewright\Documents\Code\R\imdccal\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1311" documentId="8_{A754B7F6-7D3D-4F69-92F9-D4031A51AC3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7805047E-D623-4252-B826-6B56F2BCF206}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5DD1C5A-4D56-4D40-8D9C-93A7BE639718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3840" yWindow="3840" windowWidth="23040" windowHeight="12120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SPAC Information" sheetId="1" r:id="rId1"/>
     <sheet name="SPAC Data" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="OLE_LINK5" localSheetId="0">'SPAC Information'!$A$71</definedName>
+    <definedName name="OLE_LINK5" localSheetId="0">'SPAC Information'!$A$69</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'SPAC Data'!$A:$A,'SPAC Data'!$4:$4</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'SPAC Information'!$29:$29</definedName>
   </definedNames>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="236">
   <si>
     <t>CCAL Water Analysis Laboratory</t>
   </si>
@@ -756,9 +756,6 @@
   </si>
   <si>
     <t>Concentration of total dissolved nitrogen for samples # 19, 23-25, 30, 31, 35, 36, 40 &amp; 44 is greater than total nitrogen. Results fall outside the normal limits of variability and do not meet Data Quality Objectives.  Reanalyses were performed with consistent results. All internal quality assurance parameters for all analytical sets were within precision limits, and all other results were valid.</t>
-  </si>
-  <si>
-    <t>Concentration of total dissolved nitrogen for samples # 21, 23, 36, 38, 39 &amp; 44 is greater than total nitrogen.  Results fall within precision limits; the results are analytically equal.</t>
   </si>
   <si>
     <t>1.45</t>
@@ -1301,41 +1298,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E75"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69:XFD70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.453125" customWidth="1"/>
-    <col min="2" max="2" width="17.26953125" style="14" customWidth="1"/>
-    <col min="3" max="3" width="28.26953125" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.1796875" style="14"/>
+    <col min="1" max="1" width="23.44140625" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" style="14" customWidth="1"/>
+    <col min="3" max="3" width="28.21875" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.21875" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>120</v>
       </c>
@@ -1343,47 +1340,47 @@
         <v>225</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="28" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>9</v>
       </c>
@@ -1397,17 +1394,17 @@
       <c r="D22" s="29"/>
       <c r="E22" s="29"/>
     </row>
-    <row r="24" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>12</v>
       </c>
@@ -1424,7 +1421,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>16</v>
       </c>
@@ -1441,7 +1438,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>17</v>
       </c>
@@ -1458,7 +1455,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>18</v>
       </c>
@@ -1475,7 +1472,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>19</v>
       </c>
@@ -1492,7 +1489,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>20</v>
       </c>
@@ -1509,7 +1506,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>21</v>
       </c>
@@ -1526,7 +1523,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>22</v>
       </c>
@@ -1543,7 +1540,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>23</v>
       </c>
@@ -1560,7 +1557,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>24</v>
       </c>
@@ -1577,7 +1574,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>25</v>
       </c>
@@ -1594,7 +1591,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>26</v>
       </c>
@@ -1611,7 +1608,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>27</v>
       </c>
@@ -1628,7 +1625,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>28</v>
       </c>
@@ -1645,7 +1642,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>29</v>
       </c>
@@ -1662,7 +1659,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>30</v>
       </c>
@@ -1679,7 +1676,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>31</v>
       </c>
@@ -1696,7 +1693,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>32</v>
       </c>
@@ -1713,7 +1710,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>33</v>
       </c>
@@ -1730,7 +1727,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>34</v>
       </c>
@@ -1747,7 +1744,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>35</v>
       </c>
@@ -1764,7 +1761,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>36</v>
       </c>
@@ -1781,7 +1778,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>37</v>
       </c>
@@ -1798,7 +1795,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>38</v>
       </c>
@@ -1815,7 +1812,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>39</v>
       </c>
@@ -1832,7 +1829,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>40</v>
       </c>
@@ -1849,7 +1846,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>41</v>
       </c>
@@ -1866,7 +1863,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>42</v>
       </c>
@@ -1883,7 +1880,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>43</v>
       </c>
@@ -1900,7 +1897,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>44</v>
       </c>
@@ -1917,7 +1914,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>45</v>
       </c>
@@ -1934,12 +1931,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>8</v>
       </c>
@@ -1971,52 +1968,42 @@
       <c r="D67" s="31"/>
       <c r="E67" s="31"/>
     </row>
-    <row r="69" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="30" t="s">
-        <v>231</v>
+    <row r="69" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="31" t="s">
+        <v>121</v>
       </c>
       <c r="B69" s="31"/>
       <c r="C69" s="31"/>
       <c r="D69" s="31"/>
       <c r="E69" s="31"/>
     </row>
-    <row r="71" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="31" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B71" s="31"/>
       <c r="C71" s="31"/>
       <c r="D71" s="31"/>
       <c r="E71" s="31"/>
     </row>
-    <row r="73" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="31" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B73" s="31"/>
       <c r="C73" s="31"/>
       <c r="D73" s="31"/>
       <c r="E73" s="31"/>
     </row>
-    <row r="75" spans="1:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="31" t="s">
-        <v>123</v>
-      </c>
-      <c r="B75" s="31"/>
-      <c r="C75" s="31"/>
-      <c r="D75" s="31"/>
-      <c r="E75" s="31"/>
-    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="7">
     <mergeCell ref="A22:E22"/>
     <mergeCell ref="A63:E63"/>
     <mergeCell ref="A65:E65"/>
     <mergeCell ref="A67:E67"/>
-    <mergeCell ref="A75:E75"/>
+    <mergeCell ref="A73:E73"/>
     <mergeCell ref="A69:E69"/>
     <mergeCell ref="A71:E71"/>
-    <mergeCell ref="A73:E73"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2037,19 +2024,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.54296875" style="4" customWidth="1"/>
-    <col min="2" max="3" width="10.26953125" style="14" customWidth="1"/>
-    <col min="4" max="4" width="17.1796875" style="14" customWidth="1"/>
+    <col min="1" max="1" width="15.5546875" style="4" customWidth="1"/>
+    <col min="2" max="3" width="10.21875" style="14" customWidth="1"/>
+    <col min="4" max="4" width="17.21875" style="14" customWidth="1"/>
     <col min="5" max="5" width="30" style="14" customWidth="1"/>
-    <col min="6" max="6" width="12.08984375" style="14" customWidth="1"/>
-    <col min="7" max="8" width="10.26953125" style="14" customWidth="1"/>
-    <col min="9" max="9" width="11.26953125" style="14" customWidth="1"/>
-    <col min="10" max="66" width="10.26953125" style="14" customWidth="1"/>
+    <col min="6" max="6" width="12.109375" style="14" customWidth="1"/>
+    <col min="7" max="8" width="10.21875" style="14" customWidth="1"/>
+    <col min="9" max="9" width="11.21875" style="14" customWidth="1"/>
+    <col min="10" max="66" width="10.21875" style="14" customWidth="1"/>
     <col min="67" max="67" width="105" style="22" customWidth="1"/>
-    <col min="68" max="258" width="10.26953125" customWidth="1"/>
+    <col min="68" max="258" width="10.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:67" s="6" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:67" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2120,7 +2107,7 @@
       <c r="BN1" s="16"/>
       <c r="BO1" s="19"/>
     </row>
-    <row r="2" spans="1:67" s="6" customFormat="1" ht="14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:67" s="6" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>20</v>
       </c>
@@ -2191,7 +2178,7 @@
       <c r="BN2" s="16"/>
       <c r="BO2" s="19"/>
     </row>
-    <row r="3" spans="1:67" s="8" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:67" s="8" customFormat="1" ht="28.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>217</v>
       </c>
@@ -2262,7 +2249,7 @@
       <c r="BN3" s="17"/>
       <c r="BO3" s="20"/>
     </row>
-    <row r="4" spans="1:67" s="10" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:67" s="10" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>21</v>
       </c>
@@ -2465,7 +2452,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:67" s="13" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:67" s="13" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>156</v>
       </c>
@@ -2473,7 +2460,7 @@
         <v>155</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>186</v>
@@ -2632,7 +2619,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:67" s="13" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:67" s="13" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>157</v>
       </c>
@@ -2779,7 +2766,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:67" s="13" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:67" s="13" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>158</v>
       </c>
@@ -2926,7 +2913,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:67" s="13" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:67" s="13" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>159</v>
       </c>
@@ -2964,7 +2951,7 @@
         <v>72979</v>
       </c>
       <c r="M8" s="26" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="N8" s="26" t="s">
         <v>221</v>
@@ -3081,7 +3068,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:67" s="13" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:67" s="13" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>160</v>
       </c>
@@ -3211,7 +3198,7 @@
         <v>72969</v>
       </c>
       <c r="BE9" s="26" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="BF9" s="26" t="s">
         <v>220</v>
@@ -3231,7 +3218,7 @@
         <v>72969</v>
       </c>
       <c r="BM9" s="26" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="BN9" s="26" t="s">
         <v>220</v>
@@ -3240,7 +3227,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:67" s="13" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:67" s="13" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>161</v>
       </c>
@@ -3383,7 +3370,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="11" spans="1:67" s="13" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:67" s="13" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>162</v>
       </c>
@@ -3526,7 +3513,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:67" s="13" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:67" s="13" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>163</v>
       </c>
@@ -3685,7 +3672,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:67" s="13" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:67" s="13" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>164</v>
       </c>
@@ -3840,7 +3827,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:67" s="13" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:67" s="13" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>165</v>
       </c>
@@ -3991,7 +3978,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:67" s="13" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:67" s="13" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>166</v>
       </c>
@@ -4150,7 +4137,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:67" s="13" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:67" s="13" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>167</v>
       </c>
@@ -4297,7 +4284,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:67" s="13" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:67" s="13" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>168</v>
       </c>
@@ -4444,7 +4431,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:67" s="13" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:67" s="13" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>169</v>
       </c>
@@ -4591,7 +4578,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:67" s="13" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:67" s="13" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>170</v>
       </c>
@@ -4758,7 +4745,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:67" s="13" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:67" s="13" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>171</v>
       </c>
@@ -4856,7 +4843,7 @@
         <v>72959</v>
       </c>
       <c r="AO20" s="26" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="AP20" s="26" t="s">
         <v>219</v>
@@ -4921,7 +4908,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:67" s="13" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:67" s="13" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>172</v>
       </c>
@@ -5072,7 +5059,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:67" s="13" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:67" s="13" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>173</v>
       </c>
@@ -5215,7 +5202,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:67" s="13" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:67" s="13" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>174</v>
       </c>
@@ -5358,7 +5345,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:67" s="13" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:67" s="13" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>175</v>
       </c>
@@ -5509,7 +5496,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="1:67" s="13" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:67" s="13" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
         <v>176</v>
       </c>
@@ -5688,7 +5675,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:67" s="13" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:67" s="13" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>177</v>
       </c>
@@ -5847,7 +5834,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="27" spans="1:67" s="13" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:67" s="13" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>178</v>
       </c>
@@ -6002,7 +5989,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:67" s="13" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:67" s="13" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>179</v>
       </c>
@@ -6149,7 +6136,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:67" s="13" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:67" s="13" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>180</v>
       </c>
@@ -6312,7 +6299,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:67" s="13" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:67" s="13" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>181</v>
       </c>
@@ -6455,7 +6442,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:67" s="13" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:67" s="13" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>182</v>
       </c>
@@ -6602,7 +6589,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="32" spans="1:67" s="13" customFormat="1" ht="25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:67" s="13" customFormat="1" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>183</v>
       </c>
@@ -6745,7 +6732,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="33" spans="1:67" s="13" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:67" s="13" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>184</v>
       </c>
@@ -6892,7 +6879,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:67" s="13" customFormat="1" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:67" s="13" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>185</v>
       </c>
@@ -7031,7 +7018,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:67" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:67" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
@@ -7098,7 +7085,7 @@
       <c r="BM35" s="3"/>
       <c r="BN35" s="3"/>
     </row>
-    <row r="36" spans="1:67" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:67" ht="13.2" x14ac:dyDescent="0.25">
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>

</xml_diff>